<commit_message>
Agregar nuevo proyecto de UiPath
</commit_message>
<xml_diff>
--- a/config/Config.xlsx
+++ b/config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Uipath_RPA_CristianAzana\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CB9A25-1E02-4C4B-B0DD-30E265E9DFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B78DD5-5847-4868-ACEE-6BA32459BE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -51,12 +51,6 @@
     <t>C:\RPA\Uipath_RPA_CristianAzana\logs\logs.txt</t>
   </si>
   <si>
-    <t>libro1</t>
-  </si>
-  <si>
-    <t>C:\RPA\Uipath_RPA_CristianAzana\salida\Libro1.xlsx</t>
-  </si>
-  <si>
     <t>archivo donde se almacenara los registros del proceso</t>
   </si>
   <si>
@@ -69,10 +63,43 @@
     <t>C:\RPA\Uipath_RPA_CristianAzana\salida\</t>
   </si>
   <si>
-    <t>file_salida</t>
+    <t>Mail de donde se enviara el correo se debe cambiar por la cuenta a utilizar: xxxxxx@xxxxxx.xx</t>
   </si>
   <si>
-    <t>Mail de donde se enviara el correo se debe cambiar por la cuenta a utilizar: xxxxxx@xxxxxx.xx</t>
+    <t>fileSalida</t>
+  </si>
+  <si>
+    <t>https://micnt.com.ec/cntapp/guia104/php/guia_cntat.php?hflagsubmit=0&amp;cmbcriterio=3&amp;cmbprov2=17&amp;txtusuarioapellido=&amp;txtusuarionombre=&amp;captchaSelection=</t>
+  </si>
+  <si>
+    <t>web_URL</t>
+  </si>
+  <si>
+    <t>url del navegador</t>
+  </si>
+  <si>
+    <t>rerunMaxCount</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>numero maximo de intentos</t>
+  </si>
+  <si>
+    <t>inicio del contador</t>
+  </si>
+  <si>
+    <t>fileExcel</t>
+  </si>
+  <si>
+    <t>C:\RPA\Uipath_RPA_CristianAzana\salida\Libro.xlsx</t>
+  </si>
+  <si>
+    <t>fileArchivo</t>
+  </si>
+  <si>
+    <t>C:\RPA\Uipath_RPA_CristianAzana\archivo\</t>
   </si>
 </sst>
 </file>
@@ -458,16 +485,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z949"/>
+  <dimension ref="A1:Z948"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" style="3" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" style="3" customWidth="1"/>
     <col min="27" max="16384" width="14.42578125" style="3"/>
@@ -513,10 +540,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -527,32 +554,47 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1493,7 +1535,6 @@
     <row r="946" ht="14.25" customHeight="1"/>
     <row r="947" ht="14.25" customHeight="1"/>
     <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -1508,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z969"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1554,8 +1595,28 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2532,8 +2593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343A132E-A7FE-4F0D-8CB5-9473FE50E93E}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>